<commit_message>
Tävling Jälla april 2023
</commit_message>
<xml_diff>
--- a/mallar/import/Jälla 2023 april/extr2_2023jälla.xlsx
+++ b/mallar/import/Jälla 2023 april/extr2_2023jälla.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\episerver\voltige\VoltigeClosedXML\mallar\import\Jälla 2023 april\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B08C4132-6F6B-46A8-8701-1F42AC0DD0AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF9E6706-907C-43EA-90CE-0B7811625768}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43200" yWindow="5430" windowWidth="14850" windowHeight="21000" tabRatio="483" activeTab="5" xr2:uid="{9C6C5895-3CBC-495A-8EC3-24DF642F0EB2}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" tabRatio="483" xr2:uid="{9C6C5895-3CBC-495A-8EC3-24DF642F0EB2}"/>
   </bookViews>
   <sheets>
     <sheet name="ekipage" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="229">
   <si>
     <t>Linda Jenvall</t>
   </si>
@@ -640,9 +640,6 @@
     <t>Vit 10</t>
   </si>
   <si>
-    <t>Vit 2</t>
-  </si>
-  <si>
     <t>Svart 11</t>
   </si>
   <si>
@@ -719,6 +716,15 @@
   </si>
   <si>
     <t>Vit 16</t>
+  </si>
+  <si>
+    <t>Vit 20</t>
+  </si>
+  <si>
+    <t>Vit 21</t>
+  </si>
+  <si>
+    <t>Linn Odensten</t>
   </si>
 </sst>
 </file>
@@ -1090,10 +1096,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73B3B0E3-2027-4083-B582-AAB0C4C3F786}">
-  <dimension ref="A1:W46"/>
+  <dimension ref="A1:W44"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:XFD25"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1400,13 +1406,13 @@
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A6">
-        <v>619327</v>
+        <v>619326</v>
       </c>
       <c r="B6">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D6">
         <v>40552</v>
@@ -1414,23 +1420,23 @@
       <c r="E6" t="s">
         <v>10</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="5">
         <v>106742</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="5" t="s">
         <v>14</v>
       </c>
       <c r="H6">
-        <v>223</v>
+        <v>869</v>
       </c>
       <c r="I6" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="L6">
-        <v>69830</v>
+        <v>106236</v>
       </c>
       <c r="M6" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.45">
@@ -1508,13 +1514,13 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A9">
-        <v>619326</v>
+        <v>619327</v>
       </c>
       <c r="B9">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D9">
         <v>40552</v>
@@ -1529,16 +1535,16 @@
         <v>189</v>
       </c>
       <c r="H9">
-        <v>869</v>
+        <v>223</v>
       </c>
       <c r="I9" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="L9">
-        <v>106236</v>
+        <v>69830</v>
       </c>
       <c r="M9" t="s">
-        <v>51</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.45">
@@ -2165,13 +2171,13 @@
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A27">
-        <v>619329</v>
+        <v>619327</v>
       </c>
       <c r="B27">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C27" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D27">
         <v>40552</v>
@@ -2179,11 +2185,11 @@
       <c r="E27" t="s">
         <v>10</v>
       </c>
-      <c r="F27" s="5">
-        <v>999</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>189</v>
+      <c r="F27">
+        <v>133740</v>
+      </c>
+      <c r="G27" t="s">
+        <v>11</v>
       </c>
       <c r="H27">
         <v>869</v>
@@ -2192,21 +2198,21 @@
         <v>12</v>
       </c>
       <c r="L27">
-        <v>145535</v>
+        <v>162160</v>
       </c>
       <c r="M27" t="s">
-        <v>136</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A28">
-        <v>619327</v>
+        <v>619329</v>
       </c>
       <c r="B28">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C28" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D28">
         <v>40552</v>
@@ -2221,119 +2227,149 @@
         <v>11</v>
       </c>
       <c r="H28">
-        <v>869</v>
+        <v>223</v>
       </c>
       <c r="I28" t="s">
-        <v>12</v>
+        <v>2</v>
+      </c>
+      <c r="J28" t="s">
+        <v>128</v>
       </c>
       <c r="L28">
-        <v>162160</v>
+        <v>150091</v>
       </c>
       <c r="M28" t="s">
-        <v>50</v>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A29">
-        <v>619329</v>
+        <v>619333</v>
       </c>
       <c r="B29">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C29" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="D29">
-        <v>40552</v>
+        <v>24976</v>
       </c>
       <c r="E29" t="s">
-        <v>10</v>
+        <v>99</v>
       </c>
       <c r="F29">
-        <v>133740</v>
+        <v>37075</v>
       </c>
       <c r="G29" t="s">
-        <v>11</v>
+        <v>92</v>
       </c>
       <c r="H29">
-        <v>223</v>
+        <v>1330</v>
       </c>
       <c r="I29" t="s">
-        <v>2</v>
+        <v>59</v>
       </c>
       <c r="J29" t="s">
-        <v>128</v>
+        <v>129</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>154</v>
       </c>
       <c r="L29">
-        <v>150091</v>
+        <v>155903</v>
       </c>
       <c r="M29" t="s">
-        <v>5</v>
+        <v>71</v>
+      </c>
+      <c r="N29">
+        <v>155915</v>
+      </c>
+      <c r="O29" t="s">
+        <v>68</v>
+      </c>
+      <c r="P29">
+        <v>128938</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>69</v>
+      </c>
+      <c r="R29">
+        <v>150829</v>
+      </c>
+      <c r="S29" t="s">
+        <v>72</v>
+      </c>
+      <c r="T29">
+        <v>164696</v>
+      </c>
+      <c r="U29" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A30">
-        <v>619333</v>
+        <v>619338</v>
       </c>
       <c r="B30">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C30" t="s">
-        <v>113</v>
+        <v>20</v>
       </c>
       <c r="D30">
-        <v>24976</v>
+        <v>40299</v>
       </c>
       <c r="E30" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F30">
-        <v>37075</v>
+        <v>176321</v>
       </c>
       <c r="G30" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H30">
-        <v>1330</v>
+        <v>984</v>
       </c>
       <c r="I30" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J30" t="s">
-        <v>129</v>
-      </c>
-      <c r="K30" s="2" t="s">
-        <v>154</v>
+        <v>130</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>155</v>
       </c>
       <c r="L30">
-        <v>155903</v>
+        <v>172145</v>
       </c>
       <c r="M30" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="N30">
-        <v>155915</v>
+        <v>186751</v>
       </c>
       <c r="O30" t="s">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="P30">
-        <v>128938</v>
+        <v>186781</v>
       </c>
       <c r="Q30" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="R30">
-        <v>150829</v>
+        <v>186646</v>
       </c>
       <c r="S30" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="T30">
-        <v>164696</v>
+        <v>186744</v>
       </c>
       <c r="U30" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.45">
@@ -2347,176 +2383,146 @@
         <v>20</v>
       </c>
       <c r="D31">
-        <v>40299</v>
+        <v>123544</v>
       </c>
       <c r="E31" t="s">
-        <v>100</v>
+        <v>147</v>
       </c>
       <c r="F31">
-        <v>176321</v>
+        <v>120448</v>
       </c>
       <c r="G31" t="s">
-        <v>93</v>
+        <v>145</v>
       </c>
       <c r="H31">
-        <v>984</v>
+        <v>223</v>
       </c>
       <c r="I31" t="s">
-        <v>60</v>
+        <v>2</v>
       </c>
       <c r="J31" t="s">
-        <v>130</v>
-      </c>
-      <c r="K31" s="3" t="s">
-        <v>155</v>
+        <v>149</v>
+      </c>
+      <c r="K31" s="4" t="s">
+        <v>149</v>
       </c>
       <c r="L31">
-        <v>172145</v>
+        <v>171787</v>
       </c>
       <c r="M31" t="s">
-        <v>73</v>
+        <v>137</v>
       </c>
       <c r="N31">
-        <v>186751</v>
+        <v>168291</v>
       </c>
       <c r="O31" t="s">
-        <v>39</v>
+        <v>138</v>
       </c>
       <c r="P31">
-        <v>186781</v>
+        <v>177906</v>
       </c>
       <c r="Q31" t="s">
-        <v>74</v>
-      </c>
-      <c r="R31">
-        <v>186646</v>
-      </c>
-      <c r="S31" t="s">
-        <v>75</v>
-      </c>
-      <c r="T31">
-        <v>186744</v>
-      </c>
-      <c r="U31" t="s">
-        <v>77</v>
+        <v>139</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A32">
-        <v>619338</v>
+        <v>619339</v>
       </c>
       <c r="B32">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C32" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D32">
-        <v>123544</v>
+        <v>39667</v>
       </c>
       <c r="E32" t="s">
-        <v>147</v>
+        <v>101</v>
       </c>
       <c r="F32">
-        <v>120448</v>
+        <v>193791</v>
       </c>
       <c r="G32" t="s">
-        <v>145</v>
+        <v>94</v>
       </c>
       <c r="H32">
-        <v>223</v>
+        <v>984</v>
       </c>
       <c r="I32" t="s">
-        <v>2</v>
+        <v>60</v>
       </c>
       <c r="J32" t="s">
-        <v>149</v>
-      </c>
-      <c r="K32" s="4" t="s">
-        <v>149</v>
+        <v>131</v>
+      </c>
+      <c r="K32" s="5" t="s">
+        <v>156</v>
       </c>
       <c r="L32">
-        <v>171787</v>
+        <v>155124</v>
       </c>
       <c r="M32" t="s">
-        <v>137</v>
+        <v>78</v>
       </c>
       <c r="N32">
-        <v>168291</v>
+        <v>171749</v>
       </c>
       <c r="O32" t="s">
-        <v>138</v>
+        <v>79</v>
       </c>
       <c r="P32">
-        <v>177906</v>
+        <v>172071</v>
       </c>
       <c r="Q32" t="s">
-        <v>139</v>
+        <v>80</v>
+      </c>
+      <c r="R32">
+        <v>134303</v>
+      </c>
+      <c r="S32" t="s">
+        <v>81</v>
+      </c>
+      <c r="T32">
+        <v>186749</v>
+      </c>
+      <c r="U32" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A33">
-        <v>619339</v>
+        <v>619340</v>
       </c>
       <c r="B33">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C33" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D33">
-        <v>39667</v>
+        <v>40552</v>
       </c>
       <c r="E33" t="s">
-        <v>101</v>
+        <v>10</v>
       </c>
       <c r="F33">
-        <v>193791</v>
+        <v>133740</v>
       </c>
       <c r="G33" t="s">
-        <v>94</v>
+        <v>11</v>
       </c>
       <c r="H33">
-        <v>984</v>
+        <v>869</v>
       </c>
       <c r="I33" t="s">
-        <v>60</v>
-      </c>
-      <c r="J33" t="s">
-        <v>131</v>
-      </c>
-      <c r="K33" s="5" t="s">
-        <v>156</v>
+        <v>12</v>
       </c>
       <c r="L33">
-        <v>155124</v>
+        <v>172585</v>
       </c>
       <c r="M33" t="s">
-        <v>78</v>
-      </c>
-      <c r="N33">
-        <v>171749</v>
-      </c>
-      <c r="O33" t="s">
-        <v>79</v>
-      </c>
-      <c r="P33">
-        <v>172071</v>
-      </c>
-      <c r="Q33" t="s">
-        <v>80</v>
-      </c>
-      <c r="R33">
-        <v>134303</v>
-      </c>
-      <c r="S33" t="s">
-        <v>81</v>
-      </c>
-      <c r="T33">
-        <v>186749</v>
-      </c>
-      <c r="U33" t="s">
-        <v>82</v>
+        <v>140</v>
       </c>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.45">
@@ -2530,28 +2536,28 @@
         <v>24</v>
       </c>
       <c r="D34">
-        <v>40552</v>
+        <v>49704</v>
       </c>
       <c r="E34" t="s">
-        <v>10</v>
+        <v>98</v>
       </c>
       <c r="F34">
-        <v>133740</v>
+        <v>180116</v>
       </c>
       <c r="G34" t="s">
-        <v>11</v>
+        <v>90</v>
       </c>
       <c r="H34">
-        <v>869</v>
+        <v>1198</v>
       </c>
       <c r="I34" t="s">
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="L34">
-        <v>172585</v>
+        <v>181877</v>
       </c>
       <c r="M34" t="s">
-        <v>140</v>
+        <v>83</v>
       </c>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.45">
@@ -2565,28 +2571,31 @@
         <v>24</v>
       </c>
       <c r="D35">
-        <v>49704</v>
+        <v>39667</v>
       </c>
       <c r="E35" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="F35">
-        <v>180116</v>
+        <v>132102</v>
       </c>
       <c r="G35" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="H35">
-        <v>1198</v>
+        <v>984</v>
       </c>
       <c r="I35" t="s">
-        <v>52</v>
+        <v>60</v>
+      </c>
+      <c r="J35" t="s">
+        <v>132</v>
       </c>
       <c r="L35">
-        <v>181877</v>
+        <v>155124</v>
       </c>
       <c r="M35" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.45">
@@ -2618,24 +2627,24 @@
         <v>60</v>
       </c>
       <c r="J36" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="L36">
-        <v>155124</v>
+        <v>172449</v>
       </c>
       <c r="M36" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A37">
-        <v>619340</v>
+        <v>619341</v>
       </c>
       <c r="B37">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C37" t="s">
-        <v>24</v>
+        <v>115</v>
       </c>
       <c r="D37">
         <v>39667</v>
@@ -2656,13 +2665,13 @@
         <v>60</v>
       </c>
       <c r="J37" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="L37">
-        <v>172449</v>
+        <v>169429</v>
       </c>
       <c r="M37" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.45">
@@ -2694,73 +2703,70 @@
         <v>60</v>
       </c>
       <c r="J38" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="L38">
-        <v>169429</v>
+        <v>169428</v>
       </c>
       <c r="M38" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A39">
-        <v>619341</v>
+        <v>619340</v>
       </c>
       <c r="B39">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C39" t="s">
-        <v>115</v>
+        <v>24</v>
       </c>
       <c r="D39">
-        <v>39667</v>
+        <v>40552</v>
       </c>
       <c r="E39" t="s">
-        <v>101</v>
+        <v>10</v>
       </c>
       <c r="F39">
-        <v>132102</v>
+        <v>133740</v>
       </c>
       <c r="G39" t="s">
-        <v>95</v>
+        <v>11</v>
       </c>
       <c r="H39">
-        <v>984</v>
+        <v>869</v>
       </c>
       <c r="I39" t="s">
-        <v>60</v>
-      </c>
-      <c r="J39" t="s">
-        <v>135</v>
+        <v>12</v>
       </c>
       <c r="L39">
-        <v>169428</v>
+        <v>182330</v>
       </c>
       <c r="M39" t="s">
-        <v>86</v>
+        <v>141</v>
       </c>
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A40">
-        <v>619340</v>
+        <v>619341</v>
       </c>
       <c r="B40">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C40" t="s">
-        <v>24</v>
-      </c>
-      <c r="D40">
+        <v>115</v>
+      </c>
+      <c r="D40" s="5">
         <v>40552</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F40">
+      <c r="F40" s="5">
         <v>133740</v>
       </c>
-      <c r="G40" t="s">
+      <c r="G40" s="5" t="s">
         <v>11</v>
       </c>
       <c r="H40">
@@ -2770,103 +2776,130 @@
         <v>12</v>
       </c>
       <c r="L40">
-        <v>182330</v>
+        <v>178065</v>
       </c>
       <c r="M40" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A41">
-        <v>619341</v>
-      </c>
-      <c r="B41">
-        <v>18</v>
-      </c>
-      <c r="C41" t="s">
-        <v>115</v>
-      </c>
-      <c r="D41">
-        <v>34557</v>
-      </c>
-      <c r="E41" t="s">
-        <v>148</v>
-      </c>
-      <c r="F41">
-        <v>17123</v>
-      </c>
-      <c r="G41" t="s">
-        <v>146</v>
-      </c>
-      <c r="H41">
-        <v>869</v>
-      </c>
-      <c r="I41" t="s">
-        <v>12</v>
-      </c>
-      <c r="L41">
-        <v>172842</v>
-      </c>
-      <c r="M41" t="s">
-        <v>143</v>
+      <c r="A41" s="5">
+        <v>101</v>
+      </c>
+      <c r="B41" s="5">
+        <v>101</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="D41" s="5">
+        <v>36847</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F41" s="5">
+        <v>81736</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H41" s="5">
+        <v>223</v>
+      </c>
+      <c r="I41" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="L41" s="5">
+        <v>1234567</v>
+      </c>
+      <c r="M41" s="5" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A42">
-        <v>619341</v>
-      </c>
-      <c r="B42">
-        <v>18</v>
-      </c>
-      <c r="C42" t="s">
-        <v>115</v>
-      </c>
-      <c r="D42">
-        <v>34557</v>
-      </c>
-      <c r="E42" t="s">
-        <v>148</v>
-      </c>
-      <c r="F42">
-        <v>17123</v>
-      </c>
-      <c r="G42" t="s">
-        <v>146</v>
-      </c>
-      <c r="H42">
-        <v>869</v>
-      </c>
-      <c r="I42" t="s">
-        <v>12</v>
-      </c>
-      <c r="L42">
-        <v>178065</v>
-      </c>
-      <c r="M42" t="s">
-        <v>144</v>
+      <c r="A42" s="5">
+        <v>102</v>
+      </c>
+      <c r="B42" s="5">
+        <v>102</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="D42" s="5">
+        <v>24976</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="F42" s="5">
+        <v>37075</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="H42" s="5">
+        <v>1330</v>
+      </c>
+      <c r="I42" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="K42" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="L42" s="5">
+        <v>2345</v>
+      </c>
+      <c r="M42" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="N42" s="5">
+        <v>345</v>
+      </c>
+      <c r="O42" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="P42" s="5">
+        <v>45</v>
+      </c>
+      <c r="Q42" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="R42" s="5">
+        <v>5</v>
+      </c>
+      <c r="S42" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="T42" s="5">
+        <v>6</v>
+      </c>
+      <c r="U42" s="5" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A43" s="5">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B43" s="5">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>161</v>
+        <v>178</v>
       </c>
       <c r="D43" s="5">
-        <v>36847</v>
+        <v>123544</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>0</v>
+        <v>147</v>
       </c>
       <c r="F43" s="5">
-        <v>81736</v>
+        <v>120448</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>1</v>
+        <v>145</v>
       </c>
       <c r="H43" s="5">
         <v>223</v>
@@ -2874,191 +2907,94 @@
       <c r="I43" s="5" t="s">
         <v>2</v>
       </c>
+      <c r="K43" s="5" t="s">
+        <v>188</v>
+      </c>
       <c r="L43" s="5">
-        <v>1234567</v>
+        <v>7</v>
       </c>
       <c r="M43" s="5" t="s">
-        <v>176</v>
+        <v>185</v>
+      </c>
+      <c r="N43" s="5">
+        <v>8</v>
+      </c>
+      <c r="O43" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="P43" s="5">
+        <v>9</v>
+      </c>
+      <c r="Q43" s="5" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A44" s="5">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B44" s="5">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>177</v>
+        <v>157</v>
       </c>
       <c r="D44" s="5">
-        <v>24976</v>
+        <v>36847</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>99</v>
+        <v>0</v>
       </c>
       <c r="F44" s="5">
-        <v>37075</v>
+        <v>200</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>92</v>
+        <v>158</v>
       </c>
       <c r="H44" s="5">
-        <v>1330</v>
+        <v>223</v>
       </c>
       <c r="I44" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="K44" s="5" t="s">
-        <v>179</v>
+        <v>2</v>
+      </c>
+      <c r="K44" t="s">
+        <v>159</v>
       </c>
       <c r="L44" s="5">
-        <v>2345</v>
+        <v>74165</v>
       </c>
       <c r="M44" s="5" t="s">
-        <v>180</v>
+        <v>17</v>
       </c>
       <c r="N44" s="5">
-        <v>345</v>
+        <v>69830</v>
       </c>
       <c r="O44" s="5" t="s">
-        <v>181</v>
+        <v>28</v>
       </c>
       <c r="P44" s="5">
-        <v>45</v>
+        <v>109403</v>
       </c>
       <c r="Q44" s="5" t="s">
-        <v>182</v>
+        <v>18</v>
       </c>
       <c r="R44" s="5">
-        <v>5</v>
+        <v>101580</v>
       </c>
       <c r="S44" s="5" t="s">
-        <v>183</v>
+        <v>49</v>
       </c>
       <c r="T44" s="5">
-        <v>6</v>
+        <v>145224</v>
       </c>
       <c r="U44" s="5" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A45" s="5">
-        <v>103</v>
-      </c>
-      <c r="B45" s="5">
-        <v>103</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="D45" s="5">
-        <v>123544</v>
-      </c>
-      <c r="E45" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="F45" s="5">
-        <v>120448</v>
-      </c>
-      <c r="G45" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="H45" s="5">
-        <v>223</v>
-      </c>
-      <c r="I45" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="K45" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="L45" s="5">
-        <v>7</v>
-      </c>
-      <c r="M45" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="N45" s="5">
-        <v>8</v>
-      </c>
-      <c r="O45" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="P45" s="5">
-        <v>9</v>
-      </c>
-      <c r="Q45" s="5" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A46" s="5">
-        <v>100</v>
-      </c>
-      <c r="B46" s="5">
-        <v>100</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="D46" s="5">
-        <v>36847</v>
-      </c>
-      <c r="E46" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="F46" s="5">
-        <v>200</v>
-      </c>
-      <c r="G46" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="H46" s="5">
-        <v>223</v>
-      </c>
-      <c r="I46" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="K46" t="s">
-        <v>159</v>
-      </c>
-      <c r="L46" s="5">
-        <v>74165</v>
-      </c>
-      <c r="M46" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="N46" s="5">
-        <v>69830</v>
-      </c>
-      <c r="O46" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="P46" s="5">
-        <v>109403</v>
-      </c>
-      <c r="Q46" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="R46" s="5">
-        <v>101580</v>
-      </c>
-      <c r="S46" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="T46" s="5">
-        <v>145224</v>
-      </c>
-      <c r="U46" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="V46" s="6">
-        <v>123456</v>
-      </c>
-      <c r="W46" s="5" t="s">
-        <v>160</v>
+      <c r="V44" s="5">
+        <v>90</v>
+      </c>
+      <c r="W44" s="5" t="s">
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -3070,8 +3006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA9D28CB-C6E2-4B8D-9091-1FD20615DBE1}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3143,7 +3079,7 @@
         <v>105</v>
       </c>
       <c r="D4" s="5">
-        <v>33</v>
+        <v>1076</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="5" t="s">
@@ -3161,7 +3097,7 @@
         <v>106</v>
       </c>
       <c r="D5" s="5">
-        <v>37</v>
+        <v>1077</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5" t="s">
@@ -3217,7 +3153,7 @@
         <v>109</v>
       </c>
       <c r="D8" s="5">
-        <v>37</v>
+        <v>1078</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
@@ -3932,10 +3868,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D5152B9-B788-4BDE-A1B2-C618945E4F4F}">
-  <dimension ref="A1:C80"/>
+  <dimension ref="A1:C81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="F76" sqref="F76"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A81" sqref="A81:B81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4123,7 +4059,7 @@
         <v>141</v>
       </c>
       <c r="C19" t="s">
-        <v>200</v>
+        <v>226</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.45">
@@ -4145,7 +4081,7 @@
         <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.45">
@@ -4164,7 +4100,7 @@
         <v>26</v>
       </c>
       <c r="C23" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.45">
@@ -4190,6 +4126,9 @@
       <c r="B26" t="s">
         <v>142</v>
       </c>
+      <c r="C26" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27">
@@ -4207,7 +4146,7 @@
         <v>19</v>
       </c>
       <c r="C28" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.45">
@@ -4218,7 +4157,7 @@
         <v>32</v>
       </c>
       <c r="C29" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.45">
@@ -4277,7 +4216,7 @@
         <v>6</v>
       </c>
       <c r="C36" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="15.4" x14ac:dyDescent="0.45">
@@ -4328,7 +4267,7 @@
         <v>49</v>
       </c>
       <c r="C42" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.45">
@@ -4339,7 +4278,7 @@
         <v>4</v>
       </c>
       <c r="C43" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.45">
@@ -4358,7 +4297,7 @@
         <v>85</v>
       </c>
       <c r="C45" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.45">
@@ -4369,7 +4308,7 @@
         <v>38</v>
       </c>
       <c r="C46" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.45">
@@ -4380,7 +4319,7 @@
         <v>13</v>
       </c>
       <c r="C47" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.45">
@@ -4423,7 +4362,7 @@
         <v>21</v>
       </c>
       <c r="C52" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.45">
@@ -4434,7 +4373,7 @@
         <v>83</v>
       </c>
       <c r="C53" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.45">
@@ -4445,7 +4384,7 @@
         <v>51</v>
       </c>
       <c r="C54" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.45">
@@ -4472,7 +4411,7 @@
         <v>42</v>
       </c>
       <c r="C57" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.45">
@@ -4483,7 +4422,7 @@
         <v>28</v>
       </c>
       <c r="C58" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.45">
@@ -4494,7 +4433,7 @@
         <v>84</v>
       </c>
       <c r="C59" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.45">
@@ -4505,7 +4444,7 @@
         <v>143</v>
       </c>
       <c r="C60" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.45">
@@ -4540,7 +4479,7 @@
         <v>40</v>
       </c>
       <c r="C64" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.45">
@@ -4551,7 +4490,7 @@
         <v>50</v>
       </c>
       <c r="C65" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.45">
@@ -4562,7 +4501,7 @@
         <v>18</v>
       </c>
       <c r="C66" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.45">
@@ -4573,7 +4512,7 @@
         <v>39</v>
       </c>
       <c r="C67" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.45">
@@ -4592,7 +4531,7 @@
         <v>144</v>
       </c>
       <c r="C69" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.45">
@@ -4611,7 +4550,7 @@
         <v>64</v>
       </c>
       <c r="C71" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.45">
@@ -4622,7 +4561,7 @@
         <v>16</v>
       </c>
       <c r="C72" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.45">
@@ -4633,7 +4572,7 @@
         <v>176</v>
       </c>
       <c r="C73" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.45">
@@ -4652,7 +4591,7 @@
         <v>17</v>
       </c>
       <c r="C75" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.45">
@@ -4693,6 +4632,14 @@
       </c>
       <c r="B80" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A81">
+        <v>90</v>
+      </c>
+      <c r="B81" t="s">
+        <v>228</v>
       </c>
     </row>
   </sheetData>

</xml_diff>